<commit_message>
Agregado de skills y language
</commit_message>
<xml_diff>
--- a/ferreiro_vitae_data.xlsx
+++ b/ferreiro_vitae_data.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="668" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="668" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
     <sheet name="awards" sheetId="5" r:id="rId2"/>
     <sheet name="courses" sheetId="7" r:id="rId3"/>
-    <sheet name="Teaching experience" sheetId="11" r:id="rId4"/>
-    <sheet name="Scientific management positions" sheetId="12" r:id="rId5"/>
-    <sheet name="Language and skills" sheetId="8" r:id="rId6"/>
+    <sheet name="otherCourses" sheetId="13" r:id="rId4"/>
+    <sheet name="teaching" sheetId="11" r:id="rId5"/>
+    <sheet name="management" sheetId="12" r:id="rId6"/>
+    <sheet name="skills" sheetId="8" r:id="rId7"/>
+    <sheet name="language" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="131">
   <si>
     <t>institution</t>
   </si>
@@ -43,27 +45,6 @@
     <t>level</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Javascript (d3.js)</t>
-  </si>
-  <si>
-    <t>C++</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Bash</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>AWK</t>
-  </si>
-  <si>
     <t>degree</t>
   </si>
   <si>
@@ -79,9 +60,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
@@ -128,9 +106,6 @@
   </si>
   <si>
     <t>CONICET (Argentina)</t>
-  </si>
-  <si>
-    <t>Interuniversitary Council (CIN) (Argentina)</t>
   </si>
   <si>
     <t>Fund for Scientific and Technological Research (FONCyT, Argentina)</t>
@@ -241,12 +216,6 @@
   </si>
   <si>
     <t>Scoreless.</t>
-  </si>
-  <si>
-    <t>Cladistiscs, phylosophy, theory and methods.</t>
-  </si>
-  <si>
-    <t>Score: B</t>
   </si>
   <si>
     <t>Statistics</t>
@@ -395,15 +364,6 @@
     <t>Niche and distribution modeling, with an emphasis on the use of MAXENT</t>
   </si>
   <si>
-    <t>Score: 7/10</t>
-  </si>
-  <si>
-    <t>Score: 10/10</t>
-  </si>
-  <si>
-    <t>Score: 9/10</t>
-  </si>
-  <si>
     <t>Federal University of Paraná, Brazil.</t>
   </si>
   <si>
@@ -419,9 +379,6 @@
     <t>Misiones, Argentina</t>
   </si>
   <si>
-    <t>Puntaje: 83/100</t>
-  </si>
-  <si>
     <t>R101</t>
   </si>
   <si>
@@ -473,85 +430,156 @@
     <t>September 9th-14th, 2016.</t>
   </si>
   <si>
-    <t>Duración: 45 hs. Puntaje: 9/10.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introducción a la filogeografía y el modelado de nicho. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FCEFyN, UNC. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-26 de Agosto de 2016. </t>
-  </si>
-  <si>
-    <t>Duración: 45 hs. Puntaje; 10/10.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análisis de la estructura genética de las poblaciones naturales. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-10 de Junio de 2016. </t>
-  </si>
-  <si>
-    <t>Duración: 45 hs. Puntaje: 10/10.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimación de tiempos de divergencia. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I Reunión Argentina de Biología Evolutiva (RABE). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 de Julio 2015. </t>
-  </si>
-  <si>
-    <t>Duración: 3 hs. Sin puntaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Árboles de especies en un context coalescente. </t>
-  </si>
-  <si>
-    <t>6 de Julio 2015.</t>
-  </si>
-  <si>
-    <t>Duración: 3 hs. Sin puntaje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curso Introductorio a SIG Y Teledetección. </t>
-  </si>
-  <si>
-    <t>Duración: 10 hs. Sin puntaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNC. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">26-27  de Junio de 2015. </t>
-  </si>
-  <si>
-    <t>Biotecnología.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Facultad de Ciencias Químicas, UNC. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desde Marzo a Junio de 2013. </t>
-  </si>
-  <si>
-    <t>Duración: 40 hs. Puntaje: 8/10.</t>
-  </si>
-  <si>
     <t>Undergraduate scholarship ("Estimulo a las Vocaciones Cientificas")</t>
+  </si>
+  <si>
+    <t>Lenght: 45 hs. Score: 9/10.</t>
+  </si>
+  <si>
+    <t>Lenght: 45 hs. Score: 10/10.</t>
+  </si>
+  <si>
+    <t>Lenght: 10 hs. Scoreless.</t>
+  </si>
+  <si>
+    <t>Lenght: 40 hs. Score: 8/10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 22th-26th, 2016. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 6th-10th, 2016. </t>
+  </si>
+  <si>
+    <t>Introductory course to GIS and teledetection</t>
+  </si>
+  <si>
+    <t>Analysis of the genetic structure of natural populations</t>
+  </si>
+  <si>
+    <t>Introduction to Phylogeography and Niche Modelling</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 26th-27th, 2015. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From March to June, 2013. </t>
+  </si>
+  <si>
+    <t>Lenght: 40hs. Score: 10/10</t>
+  </si>
+  <si>
+    <t>National Interuniversitary Council (CIN) (Argentina)</t>
+  </si>
+  <si>
+    <t>Lenght: 45hs. Score: B</t>
+  </si>
+  <si>
+    <t>Lenght: 40hs. Score: 9/10</t>
+  </si>
+  <si>
+    <t>Lenght: 40hs. Scoreless.</t>
+  </si>
+  <si>
+    <t>Lenght: 40hs. Score: 7/10</t>
+  </si>
+  <si>
+    <t>Lenght: 100hs. Score: 83/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i-Teams. Entrepreneurial training program and scientific-technological link </t>
+  </si>
+  <si>
+    <t>Ministry of Science and Technology, Governement of the Province of Córdoba, Argentina</t>
+  </si>
+  <si>
+    <t>From August to November, 2019</t>
+  </si>
+  <si>
+    <t>Representative of Fellows on the Board of Directors</t>
+  </si>
+  <si>
+    <t>Institute of Animal Diversity and Ecology (IDEA, CONICET-UNC)</t>
+  </si>
+  <si>
+    <t>2019-2021</t>
+  </si>
+  <si>
+    <t>Undergraduate assistant</t>
+  </si>
+  <si>
+    <t>Course: Animal Diversity 1</t>
+  </si>
+  <si>
+    <t>Fellow colaboration</t>
+  </si>
+  <si>
+    <t>2016-2018</t>
+  </si>
+  <si>
+    <t>Course: Population Genetics and Evolution</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Native language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Cladistiscs, Phylosophy, Theory and Methods.</t>
+  </si>
+  <si>
+    <t>Coding languages</t>
+  </si>
+  <si>
+    <t>R, UNIX, JavaScripit, HTML, CSS</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Softwares</t>
+  </si>
+  <si>
+    <t>QGIS, RGIS, Mendeley, GitHub</t>
+  </si>
+  <si>
+    <t>Lab Skills</t>
+  </si>
+  <si>
+    <t>DNA extraction, PCR, Primer design, Electrophoresis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -648,21 +676,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -980,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -995,53 +1025,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,79 +1101,79 @@
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F4" s="8">
         <v>2019</v>
@@ -1151,19 +1181,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="8">
         <v>2018</v>
@@ -1171,82 +1201,82 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1257,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,290 +1304,274 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1571,126 +1585,280 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="26.375" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.625" customWidth="1"/>
+    <col min="2" max="2" width="34.25" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio color headcolor en el yaml
</commit_message>
<xml_diff>
--- a/ferreiro_vitae_data.xlsx
+++ b/ferreiro_vitae_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="668" activeTab="7"/>
+    <workbookView xWindow="720" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="668" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -550,22 +550,29 @@
     <t>Softwares</t>
   </si>
   <si>
-    <t>QGIS, RGIS, Mendeley, GitHub</t>
-  </si>
-  <si>
     <t>Lab Skills</t>
   </si>
   <si>
     <t>DNA extraction, PCR, Primer design, Electrophoresis</t>
+  </si>
+  <si>
+    <t>QGIS, Mendeley, GitHub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -676,23 +683,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1000,7 +1007,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1760,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1793,16 +1800,16 @@
         <v>127</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1828,7 +1835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agregado de referencias al CV
</commit_message>
<xml_diff>
--- a/ferreiro_vitae_data.xlsx
+++ b/ferreiro_vitae_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ale_f\OneDrive - mi.unc.edu.ar\CVs_y_website\My_CV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566AD4E4-4C51-4D7E-BDDC-0DFA99E6CC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="668" activeTab="6"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="668" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -15,26 +21,19 @@
     <sheet name="management" sheetId="12" r:id="rId6"/>
     <sheet name="skills" sheetId="8" r:id="rId7"/>
     <sheet name="language" sheetId="14" r:id="rId8"/>
+    <sheet name="references" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="142">
   <si>
     <t>institution</t>
   </si>
@@ -541,9 +540,6 @@
     <t>Coding languages</t>
   </si>
   <si>
-    <t>R, UNIX, JavaScripit, HTML, CSS</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -556,13 +552,49 @@
     <t>DNA extraction, PCR, Primer design, Electrophoresis</t>
   </si>
   <si>
-    <t>QGIS, Mendeley, GitHub</t>
+    <t>QGIS, Mendeley, Zotero, Inkscape, PhotoShop, GitHub</t>
+  </si>
+  <si>
+    <t>R, UNIX, JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Prof. Marina B. Chiappero</t>
+  </si>
+  <si>
+    <t>Prof. Esteban Soibelzon</t>
+  </si>
+  <si>
+    <t>Prof. Sebastian Poljak</t>
+  </si>
+  <si>
+    <t>Institute of Animal Diversity and Ecology (IDEA; UNC, CONICET)</t>
+  </si>
+  <si>
+    <t>Southern Center for Scientific Research (CADIC; UNTDF, CONICET)</t>
+  </si>
+  <si>
+    <t>Vertebrate Paleontology Division, La Plata Museum (UNLP, CONICET)</t>
+  </si>
+  <si>
+    <t>Contact: marina.chiappero@gmail.com</t>
+  </si>
+  <si>
+    <t>Contact: esoibel@gmail.com</t>
+  </si>
+  <si>
+    <t>Contact: sebapoljak@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1007,18 +1039,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1083,11 +1115,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1293,7 +1326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1583,15 +1616,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="http://www.conservationtraining.org/"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId1" display="http://www.conservationtraining.org/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1640,7 +1673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1713,7 +1746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1764,11 +1797,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1812,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1791,25 +1824,25 @@
         <v>124</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1832,12 +1865,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1871,4 +1902,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9B6A64-B554-4A93-B10F-DD3E198E4D7D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego CV en español
</commit_message>
<xml_diff>
--- a/ferreiro_vitae_data.xlsx
+++ b/ferreiro_vitae_data.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ale_f\OneDrive - mi.unc.edu.ar\CVs_y_website\My_CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566AD4E4-4C51-4D7E-BDDC-0DFA99E6CC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AAED55-A68D-43E5-8EE8-6EEE344EC324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="668" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="668" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
-    <sheet name="awards" sheetId="5" r:id="rId2"/>
-    <sheet name="courses" sheetId="7" r:id="rId3"/>
-    <sheet name="otherCourses" sheetId="13" r:id="rId4"/>
-    <sheet name="teaching" sheetId="11" r:id="rId5"/>
-    <sheet name="management" sheetId="12" r:id="rId6"/>
-    <sheet name="skills" sheetId="8" r:id="rId7"/>
-    <sheet name="language" sheetId="14" r:id="rId8"/>
-    <sheet name="references" sheetId="15" r:id="rId9"/>
+    <sheet name="msSubmitted" sheetId="16" r:id="rId2"/>
+    <sheet name="awards" sheetId="5" r:id="rId3"/>
+    <sheet name="courses" sheetId="7" r:id="rId4"/>
+    <sheet name="otherCourses" sheetId="13" r:id="rId5"/>
+    <sheet name="teaching" sheetId="11" r:id="rId6"/>
+    <sheet name="management" sheetId="12" r:id="rId7"/>
+    <sheet name="skills" sheetId="8" r:id="rId8"/>
+    <sheet name="language" sheetId="14" r:id="rId9"/>
+    <sheet name="references" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
   <si>
     <t>institution</t>
   </si>
@@ -120,9 +121,6 @@
   </si>
   <si>
     <t>2021-2022</t>
-  </si>
-  <si>
-    <t>Title: Phylogeography and species distribucion models to define Conservation Units of the southern three-banded armadillo (Tolypeutes matacus) in Argentina. Manuscript on review.</t>
   </si>
   <si>
     <t>Title: Molecular phylogeny of the Euphractinae subfamily (Xenarthra). GPA 8.25/10</t>
@@ -590,12 +588,52 @@
   <si>
     <t>Contact: sebapoljak@hotmail.com</t>
   </si>
+  <si>
+    <r>
+      <t>Title: Phylogeography and species distribucion models to define Conservation Units of the southern three-banded armadillo (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tolypeutes matacus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>) in Argentina.</t>
+    </r>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Reconstructing the distribution of chacoan biota from current and past evidence: the case of the southern three-banded armadillo Tolypeutes matacus (Desmarest, 1804)</t>
+  </si>
+  <si>
+    <t>Journal of Mammalian Evolution</t>
+  </si>
+  <si>
+    <t>Under second round of reviews</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -692,6 +730,12 @@
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1050,7 +1094,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1093,12 +1137,12 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1110,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1163,112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9B6A64-B554-4A93-B10F-DD3E198E4D7D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6AD4C5-8466-490E-89D1-795F4CF00262}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="138.625" customWidth="1"/>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -1156,7 +1305,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,16 +1316,16 @@
         <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,7 +1339,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -1207,10 +1356,10 @@
         <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>12</v>
@@ -1227,10 +1376,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>12</v>
@@ -1247,16 +1396,16 @@
         <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1270,13 +1419,13 @@
         <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1290,7 +1439,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>12</v>
@@ -1301,22 +1450,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1325,7 +1474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1353,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -1361,257 +1510,257 @@
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
         <v>59</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
         <v>75</v>
       </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
         <v>80</v>
       </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>81</v>
-      </c>
-      <c r="E11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>86</v>
       </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1647,7 +1796,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -1655,16 +1804,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1700,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -1708,7 +1857,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1720,12 +1869,12 @@
         <v>2011</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1734,10 +1883,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
         <v>117</v>
-      </c>
-      <c r="E3" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1745,7 +1894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1771,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -1779,16 +1928,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1796,7 +1945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1812,7 +1961,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1821,28 +1970,28 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1864,7 +2013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1885,81 +2034,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
-      </c>
-      <c r="B3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9B6A64-B554-4A93-B10F-DD3E198E4D7D}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcciones en la solapa de ms submitted del cv en ingles
</commit_message>
<xml_diff>
--- a/ferreiro_vitae_data.xlsx
+++ b/ferreiro_vitae_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ale_f\OneDrive - mi.unc.edu.ar\CVs_y_website\My_CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AAED55-A68D-43E5-8EE8-6EEE344EC324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15299775-E598-4961-995E-182C3D79CA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="668" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,7 +626,7 @@
     <t>Journal of Mammalian Evolution</t>
   </si>
   <si>
-    <t>Under second round of reviews</t>
+    <t>Status: Under second round of reviews</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>